<commit_message>
System descriptions 3/5 are added, preliminary analysis table is now present
</commit_message>
<xml_diff>
--- a/comparison_chart.xlsx
+++ b/comparison_chart.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Criteria</t>
   </si>
@@ -35,9 +32,6 @@
     <t>Test case generation</t>
   </si>
   <si>
-    <t>Approach</t>
-  </si>
-  <si>
     <t>Use-case testing</t>
   </si>
   <si>
@@ -62,48 +56,18 @@
     <t>Testing level</t>
   </si>
   <si>
-    <t>Developer, provider, integrator, 3rd party, end-user</t>
-  </si>
-  <si>
     <t>functional, non-functional, integration, regression</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Automated test case generation using evolutionary algorithm</t>
-  </si>
-  <si>
-    <t>Case study</t>
-  </si>
-  <si>
-    <t>No experimental validation, real service, using synthetic services</t>
-  </si>
-  <si>
-    <t>black box vs white box</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>Top existing alternatives</t>
   </si>
   <si>
-    <t>Core of the system / Main focus</t>
-  </si>
-  <si>
-    <t>Main approach</t>
-  </si>
-  <si>
-    <t>Techniques used</t>
-  </si>
-  <si>
     <t>Repeatability</t>
   </si>
   <si>
-    <t>Performance measures/result</t>
-  </si>
-  <si>
     <t>Test case data generation</t>
   </si>
   <si>
@@ -113,13 +77,64 @@
     <t>Secondary result</t>
   </si>
   <si>
-    <t>Coverage result</t>
-  </si>
-  <si>
-    <t>Bugs found</t>
-  </si>
-  <si>
-    <t>Other features</t>
+    <t>Methodology</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>Programming language</t>
+  </si>
+  <si>
+    <t>Main contribution</t>
+  </si>
+  <si>
+    <t>3rd party applications used</t>
+  </si>
+  <si>
+    <t>Practicality</t>
+  </si>
+  <si>
+    <t>Controlled environment</t>
+  </si>
+  <si>
+    <t>CI/CD compatibility</t>
+  </si>
+  <si>
+    <t>Production ready</t>
+  </si>
+  <si>
+    <t>Novelty</t>
+  </si>
+  <si>
+    <t>Experimental validation</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Developer, provider, integrator, 3rd party, end-user, black-box, white-box</t>
+  </si>
+  <si>
+    <t>X bugs found</t>
+  </si>
+  <si>
+    <t>Coverage %</t>
+  </si>
+  <si>
+    <t>Performance measures</t>
+  </si>
+  <si>
+    <t>Size of tested environment</t>
+  </si>
+  <si>
+    <t>Small/Medium/Large</t>
+  </si>
+  <si>
+    <t>Limitations</t>
+  </si>
+  <si>
+    <t>Comparison with other tools</t>
   </si>
 </sst>
 </file>
@@ -454,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -519,15 +534,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -846,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H21"/>
+  <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,23 +878,23 @@
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -898,10 +908,10 @@
     </row>
     <row r="4" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
@@ -921,61 +931,55 @@
     <row r="6" spans="2:8" ht="54" x14ac:dyDescent="0.35">
       <c r="B6" s="10"/>
       <c r="C6" s="18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="2:8" ht="36" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="10"/>
-      <c r="C7" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>13</v>
-      </c>
+      <c r="C7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="19"/>
       <c r="E7" s="20"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="2:8" ht="54" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
-      <c r="C8" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>15</v>
-      </c>
+      <c r="C8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="19"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="2:8" ht="36.299999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="23"/>
-      <c r="C9" s="24" t="s">
-        <v>16</v>
+    <row r="9" spans="2:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="B9" s="10"/>
+      <c r="C9" s="21" t="s">
+        <v>9</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>22</v>
+    <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B10" s="10"/>
+      <c r="C10" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
@@ -983,10 +987,10 @@
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="2:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="27"/>
-      <c r="C11" s="22" t="s">
-        <v>4</v>
+    <row r="11" spans="2:8" ht="36.299999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="23"/>
+      <c r="C11" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
@@ -994,12 +998,12 @@
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="28" t="s">
-        <v>19</v>
+    <row r="12" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
@@ -1007,10 +1011,10 @@
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="10"/>
       <c r="C13" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
@@ -1018,10 +1022,10 @@
       <c r="G13" s="20"/>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
-      <c r="C14" s="22" t="s">
-        <v>18</v>
+      <c r="C14" s="27" t="s">
+        <v>25</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
@@ -1029,10 +1033,10 @@
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="10"/>
-      <c r="C15" s="22" t="s">
-        <v>21</v>
+      <c r="C15" s="27" t="s">
+        <v>12</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
@@ -1040,10 +1044,10 @@
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
     </row>
-    <row r="16" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10"/>
-      <c r="C16" s="22" t="s">
-        <v>23</v>
+      <c r="C16" s="27" t="s">
+        <v>24</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
@@ -1051,10 +1055,10 @@
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
     </row>
-    <row r="17" spans="2:8" ht="39.299999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="23"/>
-      <c r="C17" s="29" t="s">
-        <v>24</v>
+    <row r="17" spans="2:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="10"/>
+      <c r="C17" s="22" t="s">
+        <v>2</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
@@ -1062,38 +1066,123 @@
       <c r="G17" s="20"/>
       <c r="H17" s="20"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="30"/>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C19" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C20" s="1" t="s">
+    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="10"/>
+      <c r="C19" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="10"/>
+      <c r="C20" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="10"/>
+      <c r="C21" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="10"/>
+      <c r="C22" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+    </row>
+    <row r="23" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" s="10"/>
+      <c r="C23" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+    </row>
+    <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B24" s="10"/>
+      <c r="C24" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+    </row>
+    <row r="25" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B25" s="10"/>
+      <c r="C25" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="2:8" ht="39.299999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="23"/>
+      <c r="C26" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B18:B26"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
@@ -1104,8 +1193,8 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="B12:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
System description is finished
</commit_message>
<xml_diff>
--- a/comparison_chart.xlsx
+++ b/comparison_chart.xlsx
@@ -59,9 +59,6 @@
     <t>functional, non-functional, integration, regression</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>Top existing alternatives</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>CI/CD compatibility</t>
   </si>
   <si>
-    <t>Production ready</t>
-  </si>
-  <si>
     <t>Novelty</t>
   </si>
   <si>
@@ -135,6 +129,12 @@
   </si>
   <si>
     <t>Comparison with other tools</t>
+  </si>
+  <si>
+    <t>Brief description</t>
+  </si>
+  <si>
+    <t>Production readyness</t>
   </si>
 </sst>
 </file>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,10 +908,10 @@
     </row>
     <row r="4" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
@@ -934,7 +934,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6" s="20"/>
       <c r="F6" s="20"/>
@@ -944,7 +944,7 @@
     <row r="7" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="10"/>
       <c r="C7" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
@@ -955,7 +955,7 @@
     <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
       <c r="C8" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="20"/>
@@ -979,7 +979,7 @@
     <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
       <c r="C10" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
@@ -990,7 +990,7 @@
     <row r="11" spans="2:8" ht="36.299999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="12" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="26" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>23</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
@@ -1014,7 +1014,7 @@
     <row r="13" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="10"/>
       <c r="C13" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="20"/>
@@ -1025,7 +1025,7 @@
     <row r="14" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
       <c r="C14" s="27" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="20"/>
@@ -1036,7 +1036,7 @@
     <row r="15" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="10"/>
       <c r="C15" s="27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="20"/>
@@ -1047,7 +1047,7 @@
     <row r="16" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10"/>
       <c r="C16" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="20"/>
@@ -1068,7 +1068,7 @@
     </row>
     <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>1</v>
@@ -1082,10 +1082,10 @@
     <row r="19" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
       <c r="C19" s="22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
@@ -1095,10 +1095,10 @@
     <row r="20" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="10"/>
       <c r="C20" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
@@ -1108,10 +1108,10 @@
     <row r="21" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
       <c r="C21" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
@@ -1121,7 +1121,7 @@
     <row r="22" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="10"/>
       <c r="C22" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="20"/>
@@ -1132,7 +1132,7 @@
     <row r="23" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
       <c r="C23" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="19"/>
       <c r="E23" s="20"/>
@@ -1143,10 +1143,10 @@
     <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B24" s="10"/>
       <c r="C24" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
@@ -1156,7 +1156,7 @@
     <row r="25" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
       <c r="C25" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="20"/>
@@ -1167,7 +1167,7 @@
     <row r="26" spans="2:8" ht="39.299999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="23"/>
       <c r="C26" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="20"/>

</xml_diff>

<commit_message>
Comparison chart filled, first clear draft
</commit_message>
<xml_diff>
--- a/comparison_chart.xlsx
+++ b/comparison_chart.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
   <si>
     <t>Criteria</t>
   </si>
@@ -38,12 +39,6 @@
     <t>Repeatability</t>
   </si>
   <si>
-    <t>Primary result</t>
-  </si>
-  <si>
-    <t>Secondary result</t>
-  </si>
-  <si>
     <t>Methodology</t>
   </si>
   <si>
@@ -62,34 +57,16 @@
     <t>CI/CD compatibility</t>
   </si>
   <si>
-    <t>Novelty</t>
-  </si>
-  <si>
     <t>Experimental validation</t>
   </si>
   <si>
-    <t>X bugs found</t>
-  </si>
-  <si>
-    <t>Coverage %</t>
-  </si>
-  <si>
     <t>Performance measures</t>
   </si>
   <si>
-    <t>Size of tested environment</t>
-  </si>
-  <si>
-    <t>Small/Medium/Large</t>
-  </si>
-  <si>
     <t>Limitations</t>
   </si>
   <si>
     <t>Brief description</t>
-  </si>
-  <si>
-    <t>Production readyness</t>
   </si>
   <si>
     <t>Andrea Arcuri [9]</t>
@@ -150,12 +127,6 @@
     <t>C#, .NET platform</t>
   </si>
   <si>
-    <t xml:space="preserve">Swagger, IntelliJ Coverage, </t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
     <t>3rd party tools used</t>
   </si>
   <si>
@@ -168,90 +139,150 @@
     <t>Testing method (box-approach)</t>
   </si>
   <si>
-    <t>Gray-box</t>
+    <t>Functional testing</t>
+  </si>
+  <si>
+    <t>Manual effort concerns</t>
+  </si>
+  <si>
+    <t>Automatic test case generation for REST</t>
+  </si>
+  <si>
+    <t>XMI, Java</t>
+  </si>
+  <si>
+    <t>XSD, WADL, Java</t>
+  </si>
+  <si>
+    <t>Platforms/Languages</t>
+  </si>
+  <si>
+    <t>WADL++</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Existing alternatives</t>
+  </si>
+  <si>
+    <t>Limited, due to code coverage</t>
+  </si>
+  <si>
+    <t>SoapUI, Trang</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Xenu, LinkTiger, Audisto</t>
+  </si>
+  <si>
+    <t>JUnit, ArgoUML, JavaCC, JJTree, CodeModel, HttpComponents</t>
+  </si>
+  <si>
+    <t>Modelling the specific behavior of the system</t>
+  </si>
+  <si>
+    <t>SUT has to be configured manually once</t>
+  </si>
+  <si>
+    <t>Partially required</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>BaseX XML database</t>
+  </si>
+  <si>
+    <t>Misleading error rates on simple test cases</t>
+  </si>
+  <si>
+    <t>Microsoft XSD Inferencer, SoapUI, Trang</t>
+  </si>
+  <si>
+    <t>Java, Kotlin</t>
+  </si>
+  <si>
+    <t>DataGenerator</t>
+  </si>
+  <si>
+    <t>Swagger, IntelliJ Coverage, EvoSuite</t>
+  </si>
+  <si>
+    <t>Immature compared to existing alternatives</t>
+  </si>
+  <si>
+    <t>Evolution can mutate in a particular way</t>
+  </si>
+  <si>
+    <t>GraphWalker, SpecExplorer, NModel</t>
+  </si>
+  <si>
+    <t>Complexity of the tool</t>
+  </si>
+  <si>
+    <t>Writing the test cases under WADL++</t>
+  </si>
+  <si>
+    <t>Tests are given as input</t>
+  </si>
+  <si>
+    <t>1 in-house prototype project</t>
+  </si>
+  <si>
+    <t>1 internal, 1 industrial web services</t>
+  </si>
+  <si>
+    <t>2 open-source, 1 industrial web services</t>
+  </si>
+  <si>
+    <t>1 in-house web service</t>
+  </si>
+  <si>
+    <t>Not required</t>
+  </si>
+  <si>
+    <t>Comparison against other tools</t>
+  </si>
+  <si>
+    <t>Writing the test cases under proposed framework</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>176 test cases generated, 38 bugs identified. But, yielded low coverage rate.</t>
+  </si>
+  <si>
+    <t>Inferencer validated all given documents. Errors found with a 56.26% precision.</t>
+  </si>
+  <si>
+    <t>Tool genereated 16 referenced URI and raised exceptions for all.</t>
+  </si>
+  <si>
+    <t>Tool can detect bugs and generate exhaustive test cases (Inadequate quantitative data).</t>
+  </si>
+  <si>
+    <t>SpecFlow, SoapUI</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Non-functional testing, </t>
+      <t xml:space="preserve">Non-functional testing                 </t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="14"/>
+        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="162"/>
         <scheme val="minor"/>
       </rPr>
-      <t>connectedness</t>
+      <t>(connectedness)</t>
     </r>
-  </si>
-  <si>
-    <t>Functional testing</t>
-  </si>
-  <si>
-    <t>Manual effort concerns</t>
-  </si>
-  <si>
-    <t>Writing the test cases under the framework</t>
-  </si>
-  <si>
-    <t>Using their specification language describe the system</t>
-  </si>
-  <si>
-    <t>Model the specific behavior of the system</t>
-  </si>
-  <si>
-    <t>SUT has to be configured manually with the tool</t>
-  </si>
-  <si>
-    <t>2 open-source, 1 industrial</t>
-  </si>
-  <si>
-    <t>Automatic test case generation for REST</t>
-  </si>
-  <si>
-    <t>XMI, Java</t>
-  </si>
-  <si>
-    <t>XSD, WADL, Java</t>
-  </si>
-  <si>
-    <t>Platforms/Languages</t>
-  </si>
-  <si>
-    <t>WADL++</t>
-  </si>
-  <si>
-    <t>Required</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Existing alternatives</t>
-  </si>
-  <si>
-    <t>Limited, due to code coverage</t>
-  </si>
-  <si>
-    <t>Result comparison with others</t>
-  </si>
-  <si>
-    <t>SoapUI, Trang</t>
-  </si>
-  <si>
-    <t>1 internal, 1 industrial</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Xenu, LinkTiger, Audisto</t>
-  </si>
-  <si>
-    <t>SpecFlow, SoapUI,</t>
   </si>
 </sst>
 </file>
@@ -260,6 +291,15 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -284,17 +324,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="162"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
@@ -603,82 +633,82 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -993,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H27"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection sqref="A1:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,7 +1036,7 @@
     <col min="3" max="3" width="34.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.77734375" style="1" customWidth="1"/>
     <col min="7" max="7" width="28.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="29.109375" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="1"/>
@@ -1019,19 +1049,19 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1045,28 +1075,28 @@
     </row>
     <row r="4" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>28</v>
-      </c>
       <c r="G4" s="14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10"/>
       <c r="C5" s="15"/>
       <c r="D5" s="16"/>
@@ -1075,341 +1105,354 @@
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="10"/>
       <c r="C6" s="18" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="36" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="32.4" x14ac:dyDescent="0.35">
       <c r="B7" s="10"/>
       <c r="C7" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="20"/>
+        <v>37</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>37</v>
+      </c>
       <c r="H7" s="20" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
       <c r="C8" s="18" t="s">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+        <v>24</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="H8" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="10"/>
-      <c r="C9" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-    </row>
-    <row r="10" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="C9" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="36" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
       <c r="C10" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="2:8" ht="36.299999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="23"/>
       <c r="C11" s="24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+        <v>44</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>53</v>
+      </c>
       <c r="G12" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="20"/>
+        <v>71</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="10"/>
       <c r="C13" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="B14" s="10"/>
+      <c r="C14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="20" t="s">
         <v>59</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="10"/>
-      <c r="C14" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="10"/>
-      <c r="C15" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
+      <c r="C15" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>24</v>
+      </c>
       <c r="H15" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="43.65" customHeight="1" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="10"/>
-      <c r="C16" s="27" t="s">
-        <v>11</v>
+      <c r="C16" s="22" t="s">
+        <v>38</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+        <v>73</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>48</v>
+      </c>
       <c r="H16" s="20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="10"/>
-      <c r="C17" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>10</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="20"/>
+        <v>25</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="H17" s="20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B18" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-    </row>
-    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="10"/>
+      <c r="C18" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
       <c r="C19" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>25</v>
+      </c>
       <c r="F19" s="20" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B20" s="10"/>
       <c r="C20" s="22" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="10"/>
-      <c r="C21" s="22" t="s">
-        <v>5</v>
+        <v>25</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="23"/>
+      <c r="C21" s="29" t="s">
+        <v>74</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-    </row>
-    <row r="22" spans="2:8" ht="14.55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="10"/>
-      <c r="C22" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B23" s="10"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B24" s="10"/>
-      <c r="C24" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-    </row>
-    <row r="25" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B25" s="10"/>
-      <c r="C25" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" s="20"/>
-    </row>
-    <row r="26" spans="2:8" ht="39.299999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="23"/>
-      <c r="C26" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="29"/>
+        <v>78</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H2:H3"/>
-    <mergeCell ref="B18:B26"/>
+    <mergeCell ref="B17:B21"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
@@ -1421,7 +1464,7 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B11"/>
-    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="B12:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>